<commit_message>
Lots of updates all around
</commit_message>
<xml_diff>
--- a/result_tables.xlsx
+++ b/result_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Greg\Carleton\Credit_Risk_Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AF5D93F-3636-48FF-8B9D-FA164C363FF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF45890A-5774-4F63-9E4E-98965DC6162C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="721" activeTab="1" xr2:uid="{8CF92A29-1E77-48F5-8D76-6F28C9ECD380}"/>
+    <workbookView xWindow="2295" yWindow="2295" windowWidth="21600" windowHeight="11385" tabRatio="721" activeTab="1" xr2:uid="{8CF92A29-1E77-48F5-8D76-6F28C9ECD380}"/>
   </bookViews>
   <sheets>
     <sheet name="Equations" sheetId="3" r:id="rId1"/>
@@ -153,15 +153,6 @@
     <t xml:space="preserve">                   pre       rec       spe        f1       geo       iba       sup</t>
   </si>
   <si>
-    <t xml:space="preserve">          0       0.04      0.68      0.91      0.07      0.79      0.61        87</t>
-  </si>
-  <si>
-    <t xml:space="preserve">          1       1.00      0.91      0.68      0.95      0.79      0.63     17118</t>
-  </si>
-  <si>
-    <t>avg / total       0.99      0.91      0.68      0.95      0.79      0.63     17205</t>
-  </si>
-  <si>
     <t xml:space="preserve">          0       0.07      0.91      0.94      0.14      0.93      0.85        87</t>
   </si>
   <si>
@@ -217,14 +208,23 @@
   <si>
     <t>True Positive Rate (TPR or Recall)</t>
   </si>
+  <si>
+    <t xml:space="preserve">          0       0.04      0.67      0.91      0.07      0.78      0.59        87</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          1       1.00      0.91      0.67      0.95      0.78      0.62     17118</t>
+  </si>
+  <si>
+    <t>avg / total       0.99      0.91      0.67      0.95      0.78      0.62     17205</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="168" formatCode="0.0%"/>
-    <numFmt numFmtId="169" formatCode="0.000%"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="0.000%"/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
@@ -401,7 +401,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -413,15 +413,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -441,14 +435,20 @@
     <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1282,11 +1282,11 @@
       <c r="A1" s="9"/>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="12" t="s">
+      <c r="H1" s="10"/>
+      <c r="I1" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="11" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1294,13 +1294,13 @@
       <c r="A2" s="9"/>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="I2" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="15" t="s">
+      <c r="J2" s="13" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1308,43 +1308,43 @@
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="14" t="s">
+      <c r="H3" s="22"/>
+      <c r="I3" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="14" t="s">
+      <c r="J3" s="12" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H4" s="13" t="s">
+      <c r="H4" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="15" t="s">
+      <c r="I4" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="15" t="s">
+      <c r="J4" s="13" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="51" x14ac:dyDescent="0.25">
-      <c r="H5" s="13"/>
-      <c r="I5" s="14" t="s">
+      <c r="H5" s="22"/>
+      <c r="I5" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="J5" s="14" t="s">
+      <c r="J5" s="12" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H6" s="10"/>
+      <c r="H6" s="23"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H7" s="10"/>
+      <c r="H7" s="23"/>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="23" t="s">
-        <v>49</v>
+      <c r="A19" s="21" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1363,7 +1363,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="A1:D7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1454,7 +1454,7 @@
         <v>7</v>
       </c>
       <c r="D6" s="6">
-        <v>0.79599715564580098</v>
+        <v>0.78776726253066898</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -1465,7 +1465,7 @@
         <v>8</v>
       </c>
       <c r="D7" s="6">
-        <v>0.92525210405662905</v>
+        <v>0.92542735817510102</v>
       </c>
     </row>
   </sheetData>
@@ -1482,16 +1482,16 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44" customWidth="1"/>
-    <col min="2" max="2" width="12" style="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" style="21" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" style="21" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" style="21" customWidth="1"/>
+    <col min="2" max="2" width="12" style="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" style="19" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" style="19" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" style="19" customWidth="1"/>
     <col min="7" max="7" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1503,46 +1503,46 @@
         <v>21</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>48</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="20">
+      <c r="B2" s="18">
         <f>ClusterCentroids!$C$3/(ClusterCentroids!$C$3+ClusterCentroids!$C$2)</f>
         <v>0.99560098330961311</v>
       </c>
-      <c r="C2" s="20">
+      <c r="C2" s="18">
         <f>ClusterCentroids!$C$3/(ClusterCentroids!$C$3+ClusterCentroids!$B$3)</f>
         <v>0.44952681388012616</v>
       </c>
-      <c r="D2" s="20">
+      <c r="D2" s="18">
         <f>ClusterCentroids!$B$2/(ClusterCentroids!$B$2+ClusterCentroids!$C$2)</f>
         <v>0.60919540229885061</v>
       </c>
-      <c r="E2" s="20">
+      <c r="E2" s="18">
         <f>ClusterCentroids!$B$3/(ClusterCentroids!$C$3+ClusterCentroids!$B$3)</f>
         <v>0.55047318611987384</v>
       </c>
-      <c r="F2" s="22">
+      <c r="F2" s="20">
         <f>2*B2*C2/(B2+C2)</f>
         <v>0.61939067090594435</v>
       </c>
-      <c r="G2" s="22">
+      <c r="G2" s="20">
         <f>(C2+D2)/2</f>
         <v>0.52936110808948844</v>
       </c>
@@ -1551,27 +1551,27 @@
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="20">
+      <c r="B3" s="18">
         <f>SMOTE!$C$3/(SMOTE!$C$3+SMOTE!$C$2)</f>
         <v>0.9969897652016857</v>
       </c>
-      <c r="C3" s="20">
+      <c r="C3" s="18">
         <f>SMOTE!$C$3/(SMOTE!$C$3+SMOTE!$B$3)</f>
         <v>0.67718191377497372</v>
       </c>
-      <c r="D3" s="20">
+      <c r="D3" s="18">
         <f>SMOTE!$B$2/(SMOTE!$B$2+SMOTE!$C$2)</f>
         <v>0.5977011494252874</v>
       </c>
-      <c r="E3" s="20">
+      <c r="E3" s="18">
         <f>SMOTE!$B$3/(SMOTE!$C$3+SMOTE!$B$3)</f>
         <v>0.32281808622502628</v>
       </c>
-      <c r="F3" s="22">
+      <c r="F3" s="20">
         <f t="shared" ref="F3:F7" si="0">2*B3*C3/(B3+C3)</f>
         <v>0.80654026787267352</v>
       </c>
-      <c r="G3" s="22">
+      <c r="G3" s="20">
         <f t="shared" ref="G3:G7" si="1">(C3+D3)/2</f>
         <v>0.63744153160013051</v>
       </c>
@@ -1580,27 +1580,27 @@
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="20">
+      <c r="B4" s="18">
         <f>SMOTEENN!$C$3/(SMOTEENN!$C$3+SMOTEENN!$C$2)</f>
         <v>0.99737691686844232</v>
       </c>
-      <c r="C4" s="20">
+      <c r="C4" s="18">
         <f>SMOTEENN!$C$3/(SMOTEENN!$C$3+SMOTEENN!$B$3)</f>
         <v>0.57752073840401918</v>
       </c>
-      <c r="D4" s="20">
+      <c r="D4" s="18">
         <f>SMOTEENN!$B$2/(SMOTEENN!$B$2+SMOTEENN!$C$2)</f>
         <v>0.70114942528735635</v>
       </c>
-      <c r="E4" s="20">
+      <c r="E4" s="18">
         <f>SMOTEENN!$B$3/(SMOTEENN!$C$3+SMOTEENN!$B$3)</f>
         <v>0.42247926159598082</v>
       </c>
-      <c r="F4" s="22">
+      <c r="F4" s="20">
         <f t="shared" si="0"/>
         <v>0.7314835368109508</v>
       </c>
-      <c r="G4" s="22">
+      <c r="G4" s="20">
         <f t="shared" si="1"/>
         <v>0.63933508184568777</v>
       </c>
@@ -1609,27 +1609,27 @@
       <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="20">
+      <c r="B5" s="18">
         <f>RandomOverSampler!$C$3/(RandomOverSampler!$C$3+RandomOverSampler!$C$2)</f>
         <v>0.99702380952380953</v>
       </c>
-      <c r="C5" s="20">
+      <c r="C5" s="18">
         <f>RandomOverSampler!$C$3/(RandomOverSampler!$C$3+RandomOverSampler!$B$3)</f>
         <v>0.68495151302722279</v>
       </c>
-      <c r="D5" s="20">
+      <c r="D5" s="18">
         <f>RandomOverSampler!$B$2/(RandomOverSampler!$B$2+RandomOverSampler!$C$2)</f>
         <v>0.5977011494252874</v>
       </c>
-      <c r="E5" s="20">
+      <c r="E5" s="18">
         <f>RandomOverSampler!$B$3/(RandomOverSampler!$C$3+RandomOverSampler!$B$3)</f>
         <v>0.31504848697277721</v>
       </c>
-      <c r="F5" s="22">
+      <c r="F5" s="20">
         <f t="shared" si="0"/>
         <v>0.81203684465683212</v>
       </c>
-      <c r="G5" s="22">
+      <c r="G5" s="20">
         <f t="shared" si="1"/>
         <v>0.64132633122625515</v>
       </c>
@@ -1638,62 +1638,62 @@
       <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="20">
+      <c r="B6" s="18">
         <f>BalancedRandomForestClassifier!$C$3/(BalancedRandomForestClassifier!$C$3+BalancedRandomForestClassifier!$C$2)</f>
-        <v>0.99821326016208278</v>
-      </c>
-      <c r="C6" s="20">
+        <v>0.99813947520369539</v>
+      </c>
+      <c r="C6" s="18">
         <f>BalancedRandomForestClassifier!$C$3/(BalancedRandomForestClassifier!$C$3+BalancedRandomForestClassifier!$B$3)</f>
-        <v>0.91383339175137279</v>
-      </c>
-      <c r="D6" s="20">
+        <v>0.90886785839467232</v>
+      </c>
+      <c r="D6" s="18">
         <f>BalancedRandomForestClassifier!$B$2/(BalancedRandomForestClassifier!$B$2+BalancedRandomForestClassifier!$C$2)</f>
-        <v>0.67816091954022983</v>
-      </c>
-      <c r="E6" s="20">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E6" s="18">
         <f>BalancedRandomForestClassifier!$B$3/(BalancedRandomForestClassifier!$C$3+BalancedRandomForestClassifier!$B$3)</f>
-        <v>8.616660824862718E-2</v>
-      </c>
-      <c r="F6" s="22">
+        <v>9.1132141605327718E-2</v>
+      </c>
+      <c r="F6" s="20">
         <f t="shared" si="0"/>
-        <v>0.95416145658605012</v>
-      </c>
-      <c r="G6" s="22">
+        <v>0.95141415685674968</v>
+      </c>
+      <c r="G6" s="20">
         <f t="shared" si="1"/>
-        <v>0.79599715564580131</v>
+        <v>0.78776726253066953</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="20">
+      <c r="B7" s="18">
         <f>EasyEnsembleClassifier!$C$3/(EasyEnsembleClassifier!$C$3+EasyEnsembleClassifier!$C$2)</f>
-        <v>0.99950436775912277</v>
-      </c>
-      <c r="C7" s="20">
+        <v>0.99950455192915089</v>
+      </c>
+      <c r="C7" s="18">
         <f>EasyEnsembleClassifier!$C$3/(EasyEnsembleClassifier!$C$3+EasyEnsembleClassifier!$B$3)</f>
-        <v>0.94245823110176419</v>
-      </c>
-      <c r="D7" s="20">
+        <v>0.94280873933870779</v>
+      </c>
+      <c r="D7" s="18">
         <f>EasyEnsembleClassifier!$B$2/(EasyEnsembleClassifier!$B$2+EasyEnsembleClassifier!$C$2)</f>
         <v>0.90804597701149425</v>
       </c>
-      <c r="E7" s="20">
+      <c r="E7" s="18">
         <f>EasyEnsembleClassifier!$B$3/(EasyEnsembleClassifier!$C$3+EasyEnsembleClassifier!$B$3)</f>
-        <v>5.7541768898235778E-2</v>
-      </c>
-      <c r="F7" s="22">
+        <v>5.7191260661292209E-2</v>
+      </c>
+      <c r="F7" s="20">
         <f t="shared" si="0"/>
-        <v>0.97014341982621244</v>
-      </c>
-      <c r="G7" s="22">
+        <v>0.97032917480835712</v>
+      </c>
+      <c r="G7" s="20">
         <f t="shared" si="1"/>
-        <v>0.92525210405662928</v>
+        <v>0.92542735817510102</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G14" s="21"/>
+      <c r="G14" s="19"/>
     </row>
     <row r="16" spans="1:7" ht="19.5" x14ac:dyDescent="0.25">
       <c r="C16" s="8"/>
@@ -1712,73 +1712,85 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB115F0D-B0B5-4609-AC9B-115BFCDE6F99}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A6" sqref="A6:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="24" x14ac:dyDescent="0.25">
-      <c r="A1" s="16"/>
-      <c r="B1" s="16" t="s">
+    <row r="1" spans="1:7" ht="24" x14ac:dyDescent="0.25">
+      <c r="A1" s="14"/>
+      <c r="B1" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="14" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="18">
-        <v>59</v>
-      </c>
-      <c r="C2" s="18">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="B2" s="16">
+        <v>58</v>
+      </c>
+      <c r="C2" s="16">
+        <v>29</v>
+      </c>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="19">
-        <v>1475</v>
-      </c>
-      <c r="C3" s="19">
-        <v>15643</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="17">
+        <v>1560</v>
+      </c>
+      <c r="C3" s="17">
+        <v>15558</v>
+      </c>
+      <c r="E3" s="15"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E4" s="14"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1787,40 +1799,40 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="A5" sqref="A5:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" ht="24" x14ac:dyDescent="0.25">
-      <c r="A1" s="16"/>
-      <c r="B1" s="16" t="s">
+      <c r="A1" s="14"/>
+      <c r="B1" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="14" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="18">
+      <c r="B2" s="16">
         <v>79</v>
       </c>
-      <c r="C2" s="18">
+      <c r="C2" s="16">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="19">
-        <v>985</v>
-      </c>
-      <c r="C3" s="19">
-        <v>16133</v>
+      <c r="B3" s="17">
+        <v>979</v>
+      </c>
+      <c r="C3" s="17">
+        <v>16139</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1833,12 +1845,12 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1846,7 +1858,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1890,12 +1902,12 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1903,7 +1915,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1982,12 +1994,12 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1995,7 +2007,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>